<commit_message>
Inicia escrita do texto
</commit_message>
<xml_diff>
--- a/misc/tabelas-FFEB.xlsx
+++ b/misc/tabelas-FFEB.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="9270" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="9270" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="desc" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
   <si>
     <t>Método</t>
   </si>
@@ -302,13 +302,25 @@
     <t>desc_modelos</t>
   </si>
   <si>
-    <t>Tabela x – Erro Absoluto Percentual Médio (MAPE) - Fora da Amostra ( maio/2013 – dez/2014, n=20 )</t>
-  </si>
-  <si>
-    <t>Tabela x – % de vezes que modelo obteve menor MAPE em algum Estado - Fora da Amostra ( maio/2013 – dez/2014, n=20 )</t>
-  </si>
-  <si>
     <t>Tabela x – Erro Acumulado do Método com Menor MAPE (média 1-20) por Estado - Fora da Amostra ( maio/2013 – dez/2014, n=20 ) - Em Milhões</t>
+  </si>
+  <si>
+    <t>Tabela 1 – Erro Absoluto Percentual Médio (MAPE) - Fora da Amostra ( maio/2013 – dez/2014, n=20 )</t>
+  </si>
+  <si>
+    <t>Tabela 2 – % de vezes que modelo obteve menor MAPE em algum Estado - Fora da Amostra ( maio/2013 – dez/2014, n=20 )</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>1-8</t>
+  </si>
+  <si>
+    <t>1-16</t>
+  </si>
+  <si>
+    <t>1-20</t>
   </si>
 </sst>
 </file>
@@ -515,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,6 +597,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1209,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1235,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1517,19 +1532,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="9" width="11.5703125" customWidth="1"/>
+    <col min="4" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -1545,25 +1560,25 @@
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
     </row>
-    <row r="4" spans="2:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C4" s="28"/>
       <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>6</v>
+      <c r="E4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="I4" s="31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1843,6 +1858,9 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="H4:I4" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1850,13 +1868,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
     <col min="5" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
     <col min="10" max="13" width="11" customWidth="1"/>
@@ -1867,7 +1885,7 @@
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">

</xml_diff>